<commit_message>
update table object funcs
</commit_message>
<xml_diff>
--- a/supermarket_assi/data/products_template.xlsx
+++ b/supermarket_assi/data/products_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\supermarket_assi\supermarket_assi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFFFCFA-5134-4C70-B1D0-1C6E9D3378F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2558BA-A053-40BD-AD0B-D9F7595015D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Product</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Name2</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -369,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,8 +393,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -404,8 +410,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -417,6 +426,9 @@
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>